<commit_message>
Added cttv-experiment: biological activity: up/down/unknown
</commit_message>
<xml_diff>
--- a/CTTV_URI_schemes.xlsx
+++ b/CTTV_URI_schemes.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -12,14 +12,14 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$5:$D$27</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$5:$D$30</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="51">
   <si>
     <t>prefix</t>
   </si>
@@ -184,12 +184,24 @@
       <t>http://rdf.ebi.ac.uk/resource/ensembl/ENSG00000127720</t>
     </r>
   </si>
+  <si>
+    <t>cttvexp:up</t>
+  </si>
+  <si>
+    <t>cttvexp:down</t>
+  </si>
+  <si>
+    <t>cttvexp:unknown</t>
+  </si>
+  <si>
+    <t>biological_subject{properties}{activity}</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -403,7 +415,7 @@
   </cellStyles>
   <dxfs count="9">
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -418,7 +430,7 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -435,7 +447,7 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -452,7 +464,7 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right style="thin">
@@ -492,7 +504,7 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <border>
@@ -504,7 +516,7 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -518,11 +530,19 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A5:D27" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7" tableBorderDxfId="5" totalsRowBorderDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A5:D30" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7" tableBorderDxfId="5" totalsRowBorderDxfId="4">
   <tableColumns count="4">
     <tableColumn id="1" name="prefix" dataDxfId="3"/>
     <tableColumn id="2" name="namespace" dataDxfId="2"/>
@@ -576,7 +596,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -608,9 +628,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -642,6 +663,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -817,14 +839,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="52.42578125" bestFit="1" customWidth="1"/>
@@ -832,22 +854,22 @@
     <col min="4" max="4" width="73.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1"/>
-    <row r="2" spans="1:4" s="1" customFormat="1">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="1" customFormat="1">
+    <row r="3" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12"/>
     </row>
-    <row r="4" spans="1:4" s="1" customFormat="1">
+    <row r="4" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>45</v>
       </c>
       <c r="B4" s="14"/>
     </row>
-    <row r="5" spans="1:4" ht="30">
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>0</v>
       </c>
@@ -861,7 +883,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="30">
+    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
@@ -875,7 +897,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4" t="s">
@@ -885,7 +907,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>4</v>
       </c>
@@ -899,7 +921,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4" t="s">
@@ -909,7 +931,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:4" s="1" customFormat="1" ht="45">
+    <row r="10" spans="1:4" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
@@ -923,7 +945,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:4" s="1" customFormat="1" ht="45">
+    <row r="11" spans="1:4" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4" t="s">
@@ -933,7 +955,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:4" s="1" customFormat="1" ht="45">
+    <row r="12" spans="1:4" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4" t="s">
@@ -943,7 +965,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>6</v>
       </c>
@@ -957,7 +979,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -965,7 +987,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
@@ -973,7 +995,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
@@ -981,7 +1003,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
@@ -989,7 +1011,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
@@ -997,7 +1019,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
@@ -1005,7 +1027,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
@@ -1013,7 +1035,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
@@ -1021,7 +1043,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -1029,7 +1051,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -1037,7 +1059,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
@@ -1045,44 +1067,70 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
-      <c r="A25" s="2" t="s">
+    <row r="25" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="2"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="2"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="2"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B28" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C28" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D25" s="10" t="s">
+      <c r="D28" s="10" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
-      <c r="A26" s="2" t="s">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B29" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="C29" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D26" s="10" t="s">
+      <c r="D29" s="10" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="30">
-      <c r="A27" s="5"/>
-      <c r="B27" s="6"/>
-      <c r="C27" s="6" t="s">
+    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="5"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="D27" s="11" t="s">
+      <c r="D30" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="E27" s="1"/>
+      <c r="E30" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1092,9 +1140,9 @@
     <hyperlink ref="B6" r:id="rId1"/>
     <hyperlink ref="B8" r:id="rId2"/>
     <hyperlink ref="B13" r:id="rId3"/>
-    <hyperlink ref="B25" r:id="rId4"/>
+    <hyperlink ref="B28" r:id="rId4"/>
     <hyperlink ref="B10" r:id="rId5"/>
-    <hyperlink ref="B26" r:id="rId6"/>
+    <hyperlink ref="B29" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
@@ -1105,24 +1153,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
2x examples of ArrayAtlas evidence strings Added dbSNP URIs to CTTV schemes
</commit_message>
<xml_diff>
--- a/CTTV_URI_schemes.xlsx
+++ b/CTTV_URI_schemes.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -12,14 +12,14 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$5:$D$30</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$5:$D$32</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="56">
   <si>
     <t>prefix</t>
   </si>
@@ -132,9 +132,6 @@
     <t>efo:EFO_0000637</t>
   </si>
   <si>
-    <t>URI example in "evidence string" JSON file (PREFIX SYNTAX: Use the prefix followed by ":" OR FULL URI SYNTAX: namespace with field value at the end)</t>
-  </si>
-  <si>
     <t>http://www.targetvalidation.org/cttv_core</t>
   </si>
   <si>
@@ -159,32 +156,6 @@
     <t>&lt;----These 2 fields will be maintained by the CTTV core team----&gt;</t>
   </si>
   <si>
-    <r>
-      <t>ensembl:ENSG00000127720</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> OR </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>http://rdf.ebi.ac.uk/resource/ensembl/ENSG00000127720</t>
-    </r>
-  </si>
-  <si>
     <t>cttvexp:up</t>
   </si>
   <si>
@@ -195,13 +166,34 @@
   </si>
   <si>
     <t>biological_subject{properties}{activity}</t>
+  </si>
+  <si>
+    <t>dbsnp</t>
+  </si>
+  <si>
+    <t>http://identifiers.org/dbsnp/</t>
+  </si>
+  <si>
+    <t>dbsnp:rs4950929</t>
+  </si>
+  <si>
+    <t>provenance{experimental_evidence_specific}{evidence_chain}{n}{biological_subject}</t>
+  </si>
+  <si>
+    <t>provenance{experimental_evidence_specific}{evidence_chain}{n}{biological_object}</t>
+  </si>
+  <si>
+    <t>ensembl:ENSG00000127720</t>
+  </si>
+  <si>
+    <t>URI example in "evidence string" JSON file (Use the prefix &lt;Column 1&gt; followed by ":")</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -224,14 +216,6 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -368,7 +352,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -407,6 +391,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -415,7 +402,7 @@
   </cellStyles>
   <dxfs count="9">
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -430,7 +417,7 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -447,7 +434,7 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -464,7 +451,7 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right style="thin">
@@ -504,7 +491,7 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <border>
@@ -516,7 +503,7 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -542,12 +529,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A5:D30" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7" tableBorderDxfId="5" totalsRowBorderDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A5:D32" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7" tableBorderDxfId="5" totalsRowBorderDxfId="4">
   <tableColumns count="4">
     <tableColumn id="1" name="prefix" dataDxfId="3"/>
     <tableColumn id="2" name="namespace" dataDxfId="2"/>
     <tableColumn id="3" name="affected fields in &quot;evidence string&quot; json file" dataDxfId="1"/>
-    <tableColumn id="4" name="URI example in &quot;evidence string&quot; JSON file (PREFIX SYNTAX: Use the prefix followed by &quot;:&quot; OR FULL URI SYNTAX: namespace with field value at the end)" dataDxfId="0"/>
+    <tableColumn id="4" name="URI example in &quot;evidence string&quot; JSON file (Use the prefix &lt;Column 1&gt; followed by &quot;:&quot;)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -596,7 +583,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -628,10 +615,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -663,7 +649,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -839,14 +824,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="52.42578125" bestFit="1" customWidth="1"/>
@@ -854,22 +839,22 @@
     <col min="4" max="4" width="73.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="1" customFormat="1"/>
+    <row r="2" spans="1:4" s="1" customFormat="1">
       <c r="A2" s="12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="1" customFormat="1">
+      <c r="A3" s="12"/>
+    </row>
+    <row r="4" spans="1:4" s="1" customFormat="1">
+      <c r="A4" s="13" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="12"/>
-    </row>
-    <row r="4" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
-        <v>45</v>
-      </c>
       <c r="B4" s="14"/>
     </row>
-    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="30">
       <c r="A5" s="7" t="s">
         <v>0</v>
       </c>
@@ -880,10 +865,10 @@
         <v>14</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
@@ -894,10 +879,10 @@
         <v>11</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" s="2"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4" t="s">
@@ -907,7 +892,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="2" t="s">
         <v>4</v>
       </c>
@@ -921,7 +906,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="2"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4" t="s">
@@ -931,41 +916,41 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:4" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" s="1" customFormat="1" ht="45">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="D10" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="D10" s="10" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:4" s="1" customFormat="1" ht="45">
       <c r="A11" s="2"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" s="1" customFormat="1" ht="45">
       <c r="A12" s="2"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13" s="2" t="s">
         <v>6</v>
       </c>
@@ -979,7 +964,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="A14" s="2"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -987,7 +972,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="A15" s="2"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
@@ -995,7 +980,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="A16" s="2"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
@@ -1003,7 +988,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5">
       <c r="A17" s="2"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
@@ -1011,7 +996,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5">
       <c r="A18" s="2"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
@@ -1019,7 +1004,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5">
       <c r="A19" s="2"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
@@ -1027,7 +1012,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5">
       <c r="A20" s="2"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
@@ -1035,7 +1020,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5">
       <c r="A21" s="2"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
@@ -1043,7 +1028,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5">
       <c r="A22" s="2"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -1051,7 +1036,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5">
       <c r="A23" s="2"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -1059,7 +1044,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5">
       <c r="A24" s="2"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
@@ -1067,33 +1052,33 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" s="1" customFormat="1">
       <c r="A25" s="2"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" s="1" customFormat="1">
       <c r="A26" s="2"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
       <c r="D26" s="10" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" s="1" customFormat="1">
       <c r="A27" s="2"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
       <c r="D27" s="10" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
       <c r="A28" s="2" t="s">
         <v>31</v>
       </c>
@@ -1107,30 +1092,54 @@
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
+    <row r="29" spans="1:5" ht="30">
+      <c r="A29" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B29" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D29" s="11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="30">
+      <c r="A30" s="5"/>
+      <c r="B30" s="15"/>
+      <c r="C30" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D30" s="11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B31" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="C31" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D29" s="10" t="s">
+      <c r="D31" s="10" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="5"/>
-      <c r="B30" s="6"/>
-      <c r="C30" s="6" t="s">
+    <row r="32" spans="1:5" ht="30">
+      <c r="A32" s="5"/>
+      <c r="B32" s="6"/>
+      <c r="C32" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="D30" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="E30" s="1"/>
+      <c r="D32" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="E32" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1142,35 +1151,36 @@
     <hyperlink ref="B13" r:id="rId3"/>
     <hyperlink ref="B28" r:id="rId4"/>
     <hyperlink ref="B10" r:id="rId5"/>
-    <hyperlink ref="B29" r:id="rId6"/>
+    <hyperlink ref="B31" r:id="rId6"/>
+    <hyperlink ref="B29" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>
   <tableParts count="1">
-    <tablePart r:id="rId8"/>
+    <tablePart r:id="rId9"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added new cttvexp-up/down subclasses
</commit_message>
<xml_diff>
--- a/CTTV_URI_schemes.xlsx
+++ b/CTTV_URI_schemes.xlsx
@@ -12,14 +12,14 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$5:$D$32</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$5:$D$39</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="62">
   <si>
     <t>prefix</t>
   </si>
@@ -187,6 +187,24 @@
   </si>
   <si>
     <t>URI example in "evidence string" JSON file (Use the prefix &lt;Column 1&gt; followed by ":")</t>
+  </si>
+  <si>
+    <t>cttvexp:decreased_transcript_level</t>
+  </si>
+  <si>
+    <t>cttvexp:increased_transcript_level</t>
+  </si>
+  <si>
+    <t>cttvexp:decreased_translational_product_level</t>
+  </si>
+  <si>
+    <t>cttvexp:loss_of_function</t>
+  </si>
+  <si>
+    <t>cttvexp:partial_loss_of_function</t>
+  </si>
+  <si>
+    <t>cttvexp:gain_of_function</t>
   </si>
 </sst>
 </file>
@@ -386,14 +404,14 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -529,7 +547,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A5:D32" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7" tableBorderDxfId="5" totalsRowBorderDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A5:D39" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7" tableBorderDxfId="5" totalsRowBorderDxfId="4">
   <tableColumns count="4">
     <tableColumn id="1" name="prefix" dataDxfId="3"/>
     <tableColumn id="2" name="namespace" dataDxfId="2"/>
@@ -825,10 +843,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -849,10 +867,10 @@
       <c r="A3" s="12"/>
     </row>
     <row r="4" spans="1:4" s="1" customFormat="1">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="B4" s="14"/>
+      <c r="B4" s="15"/>
     </row>
     <row r="5" spans="1:4" ht="30">
       <c r="A5" s="7" t="s">
@@ -988,7 +1006,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:4">
       <c r="A17" s="2"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
@@ -996,7 +1014,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:4">
       <c r="A18" s="2"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
@@ -1004,7 +1022,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:4">
       <c r="A19" s="2"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
@@ -1012,7 +1030,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:4">
       <c r="A20" s="2"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
@@ -1020,7 +1038,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:4">
       <c r="A21" s="2"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
@@ -1028,7 +1046,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:4">
       <c r="A22" s="2"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -1036,7 +1054,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:4">
       <c r="A23" s="2"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -1044,7 +1062,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:4">
       <c r="A24" s="2"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
@@ -1052,7 +1070,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:5" s="1" customFormat="1">
+    <row r="25" spans="1:4" s="1" customFormat="1">
       <c r="A25" s="2"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4" t="s">
@@ -1062,7 +1080,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="26" spans="1:5" s="1" customFormat="1">
+    <row r="26" spans="1:4" s="1" customFormat="1">
       <c r="A26" s="2"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -1070,7 +1088,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="27" spans="1:5" s="1" customFormat="1">
+    <row r="27" spans="1:4" s="1" customFormat="1">
       <c r="A27" s="2"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
@@ -1078,68 +1096,124 @@
         <v>47</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
-      <c r="A28" s="2" t="s">
+    <row r="28" spans="1:4" s="1" customFormat="1">
+      <c r="A28" s="2"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" s="1" customFormat="1">
+      <c r="A29" s="2"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="10" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" s="1" customFormat="1">
+      <c r="A30" s="2"/>
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" s="1" customFormat="1">
+      <c r="A31" s="2"/>
+      <c r="B31" s="4"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="10" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" s="1" customFormat="1">
+      <c r="A32" s="2"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="10" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" s="1" customFormat="1">
+      <c r="A33" s="2"/>
+      <c r="B33" s="4"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="10" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" s="1" customFormat="1">
+      <c r="A34" s="2"/>
+      <c r="B34" s="4"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="10" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B35" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="C35" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D28" s="10" t="s">
+      <c r="D35" s="10" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="30">
-      <c r="A29" s="5" t="s">
+    <row r="36" spans="1:5" ht="30">
+      <c r="A36" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="B29" s="15" t="s">
+      <c r="B36" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="C29" s="6" t="s">
+      <c r="C36" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D29" s="11" t="s">
+      <c r="D36" s="11" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="30">
-      <c r="A30" s="5"/>
-      <c r="B30" s="15"/>
-      <c r="C30" s="6" t="s">
+    <row r="37" spans="1:5" ht="30">
+      <c r="A37" s="5"/>
+      <c r="B37" s="13"/>
+      <c r="C37" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="D30" s="11" t="s">
+      <c r="D37" s="11" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
-      <c r="A31" s="2" t="s">
+    <row r="38" spans="1:5">
+      <c r="A38" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B38" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C31" s="4" t="s">
+      <c r="C38" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D31" s="10" t="s">
+      <c r="D38" s="10" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="30">
-      <c r="A32" s="5"/>
-      <c r="B32" s="6"/>
-      <c r="C32" s="6" t="s">
+    <row r="39" spans="1:5" ht="30">
+      <c r="A39" s="5"/>
+      <c r="B39" s="6"/>
+      <c r="C39" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="D32" s="11" t="s">
+      <c r="D39" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="E32" s="1"/>
+      <c r="E39" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1149,10 +1223,10 @@
     <hyperlink ref="B6" r:id="rId1"/>
     <hyperlink ref="B8" r:id="rId2"/>
     <hyperlink ref="B13" r:id="rId3"/>
-    <hyperlink ref="B28" r:id="rId4"/>
+    <hyperlink ref="B35" r:id="rId4"/>
     <hyperlink ref="B10" r:id="rId5"/>
-    <hyperlink ref="B31" r:id="rId6"/>
-    <hyperlink ref="B29" r:id="rId7"/>
+    <hyperlink ref="B38" r:id="rId6"/>
+    <hyperlink ref="B36" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>

</xml_diff>